<commit_message>
Update for New Move-IN Test Cases
</commit_message>
<xml_diff>
--- a/SoutherWater_AutomationFrameWork/src/test/resources/dataSource/testdata.xlsx
+++ b/SoutherWater_AutomationFrameWork/src/test/resources/dataSource/testdata.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devesh.k\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devesh.k\git\SouthernWater\SoutherWater_AutomationFrameWork\src\test\resources\dataSource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="DashBoard" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,28 +24,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>SearchValue</t>
-  </si>
-  <si>
-    <t>JAVA</t>
-  </si>
-  <si>
-    <t>C#</t>
-  </si>
-  <si>
-    <t>Python</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>TestCase</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>kumar.devesh82@yahoo.com</t>
+  </si>
+  <si>
+    <t>Apple@123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -68,13 +82,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -353,38 +370,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update due to dashboardnew feature file and changes due to coding standard
</commit_message>
<xml_diff>
--- a/SoutherWater_AutomationFrameWork/src/test/resources/dataSource/testdata.xlsx
+++ b/SoutherWater_AutomationFrameWork/src/test/resources/dataSource/testdata.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
-    <sheet name="DashBoard" sheetId="1" r:id="rId1"/>
+    <sheet name="Dashboard" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,22 +26,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>TestCase</t>
-  </si>
-  <si>
-    <t>Dashboard</t>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Run</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>devesh.kumar@southernwater.co.uk</t>
+  </si>
+  <si>
+    <t>360@Logica</t>
   </si>
   <si>
     <t>Email</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>kumar.devesh82@yahoo.com</t>
-  </si>
-  <si>
-    <t>Apple@123</t>
   </si>
 </sst>
 </file>
@@ -65,12 +65,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -86,9 +92,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -373,36 +386,36 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.85546875" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>